<commit_message>
feat: Adicionados controles e melhorias para subri servidor e ajustes de importação de dados.
</commit_message>
<xml_diff>
--- a/backend/import.xlsx
+++ b/backend/import.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E07FFDAE-D091-4CCB-A246-437E6095B3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AA5F3A-18A7-4B05-B91C-5F2525B4E521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33990" yWindow="630" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38715" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Consignado</t>
   </si>
@@ -56,6 +59,21 @@
   </si>
   <si>
     <t>Agência Teste</t>
+  </si>
+  <si>
+    <t>Agência Azul</t>
+  </si>
+  <si>
+    <t>Capitalização</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>0002</t>
   </si>
 </sst>
 </file>
@@ -103,11 +121,12 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +475,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>46050</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>45677</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -468,89 +487,214 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>1000000</v>
+        <v>900000</v>
       </c>
       <c r="F2" s="2">
-        <v>850000</v>
+        <v>780000</v>
       </c>
       <c r="G2" s="1">
         <f>F2/E2</f>
-        <v>0.85</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>46048</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>45698</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="F3" s="2">
-        <v>410</v>
+        <v>750</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G5" si="0">F3/E3</f>
-        <v>0.82</v>
+        <f>F3/E3</f>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
+        <v>46048</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>500</v>
+      </c>
+      <c r="F4" s="2">
+        <v>410</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G10" si="0">F4/E4</f>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>46049</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>50000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>55000</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>45677</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>46050</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>900000</v>
-      </c>
-      <c r="F5" s="2">
-        <v>780000</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="E6" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>850000</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.8666666666666667</v>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>800000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>233000</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29125000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>22000</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>200</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>12000</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G5">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>